<commit_message>
File for importing models
</commit_message>
<xml_diff>
--- a/import_models/models.xlsx
+++ b/import_models/models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Activités" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="168">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -246,90 +246,96 @@
     <t xml:space="preserve">Pays</t>
   </si>
   <si>
-    <t xml:space="preserve">dhazioudha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/03/2021, à 18:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/03/2021, à 19:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/03/2021, à 17:49</t>
+    <t xml:space="preserve">Mario Kart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/04/2021, à 17:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/05/2021, à 17:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/04/2021, à 17:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salle des Morpions Liège</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cartes (5), Danse de salon (10), Football (20), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">machin (3.0), Projecteur multicouleur (10.0), Ruban adhésif (40.0), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dhaidhaiuhd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">djadjadjao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dadanda@jazoada.diod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odhaohdoahda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dazodhaoda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">djajdoaijda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babouche Boubouche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/03/2031, à 16:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/03/2031, à 22:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/03/2031, à 00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cartes (4), Danse de salon (8), Fléchettes (5), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projecteur multicouleur (30.0), Ruban adhésif (120.0), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boubouche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babouche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0499/99.99.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">super@babouche.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rue des Babouches, 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaboucheCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dkoajdoajda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/03/2041, à 21:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/06/2041, à 21:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/03/2041, à 21:19</t>
   </si>
   <si>
     <t xml:space="preserve">Hall omnisport Namur</t>
   </si>
   <si>
-    <t xml:space="preserve">Badminton (1), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dgazidha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cjezoijcze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dazho@dz.dzopd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dhgzadhazd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dahdiazh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ioazjaozjda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dapodajdada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/03/2021, à 18:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/03/2021, à 17:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/03/2021, à 17:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Badminton (2), Danse de salon (10), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Machin (25.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dhahdiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dajopdjajd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">djaodjada@dojiza.dzoj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dazohdahdoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jaozjdoazda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jdoajoda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dkoajdoajda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23/03/2041, à 21:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/06/2041, à 21:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/03/2041, à 21:19</t>
-  </si>
-  <si>
     <t xml:space="preserve">hdizhdadaz</t>
   </si>
   <si>
@@ -363,7 +369,7 @@
     <t xml:space="preserve">Badminton (10), Cartes (5), Handball (3), </t>
   </si>
   <si>
-    <t xml:space="preserve">Ruban adhésif (25.0), Projecteur multicouleur (10.0)</t>
+    <t xml:space="preserve">Ruban adhésif (25.0), Projecteur multicouleur (10.0), </t>
   </si>
   <si>
     <t xml:space="preserve">Bastin</t>
@@ -387,144 +393,6 @@
     <t xml:space="preserve">Belgique</t>
   </si>
   <si>
-    <t xml:space="preserve">Babouche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/03/2021, à 20:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/03/2021, à 19:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/03/2021, à 19:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartes (1), Badminton (2), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">machin (2.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">djoaizhjdoiahjd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jdopjdojdazjd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fjzojfofjaz@fjeo.co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dzajdoajhdoia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dkzpodkzpoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dpoazkda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fzfzefzfzfzfzfe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26/03/2021, à 12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/03/2021, à 12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/03/2021, à 12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Badminton (16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">djzpodjapodjaopdja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dzapodjapodjazp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dadanda@jazoada.diod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zdzpajdpoadada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qdzdzdzdpozkdapkda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jdazoidjaozda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mario Kart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/04/2021, à 17:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/05/2021, à 17:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/04/2021, à 17:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salle des Morpions Liège</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartes (5), Danse de salon (10), Football (20), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">machin (3.0), Projecteur multicouleur (10.0), Ruban adhésif (40.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dhaidhaiuhd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">djadjadjao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">odhaohdoahda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dazodhaoda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">djajdoaijda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Babouche Boubouche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/03/2031, à 16:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/03/2031, à 22:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/03/2031, à 00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartes (4), Danse de salon (8), Fléchettes (5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projecteur multicouleur (30.0), Ruban adhésif (120.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boubouche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0499/99.99.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">super@babouche.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rue des Babouches, 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaboucheCountry</t>
-  </si>
-  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -564,7 +432,7 @@
     <t xml:space="preserve">dajzopdajdajda</t>
   </si>
   <si>
-    <t xml:space="preserve">Danse de salon, Handball, Cartes, Football, Badminton, Paintball</t>
+    <t xml:space="preserve">Danse de salon, Handball, Cartes, Football, Badminton, Paintball, </t>
   </si>
   <si>
     <t xml:space="preserve">bastincyriel@hotmail.com</t>
@@ -594,7 +462,7 @@
     <t xml:space="preserve">Salle Jen-Jaurès Bruxelles</t>
   </si>
   <si>
-    <t xml:space="preserve">Danse de salon, Cartes, Badminton</t>
+    <t xml:space="preserve">Danse de salon, Cartes, Badminton, </t>
   </si>
   <si>
     <t xml:space="preserve">Molimo</t>
@@ -675,7 +543,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -774,20 +641,19 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="84.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="95.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,7 +667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -815,7 +681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -829,7 +695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -843,7 +709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -853,7 +719,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -867,7 +733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -881,7 +747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -895,7 +761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -928,16 +794,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="28.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,13 +810,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -959,13 +824,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -973,13 +838,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1006,24 +871,23 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -1081,7 +945,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -1110,7 +974,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1139,7 +1003,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -1184,35 +1048,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="26.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="61.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="85.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="85.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="25.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="30.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1271,7 +1134,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -1285,13 +1148,13 @@
         <v>76</v>
       </c>
       <c r="E2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>50</v>
-      </c>
       <c r="G2" s="1" t="n">
-        <v>111</v>
+        <v>111111</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>77</v>
@@ -1299,102 +1162,104 @@
       <c r="I2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>46546465464</v>
+        <v>4546544456</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>55454</v>
+        <v>45646</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>25</v>
+        <v>89.99</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1515</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N3" s="1" t="n">
-        <v>5456465464</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="1" t="n">
-        <v>4545</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="S3" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1406,48 +1271,48 @@
         <v>45</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>4564644464</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Q4" s="1" t="n">
         <v>4545</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>10</v>
@@ -1459,266 +1324,38 @@
         <v>41</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Q5" s="1" t="n">
         <v>5002</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>444454654644</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q6" s="1" t="n">
-        <v>1111</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="N7" s="1" t="n">
-        <v>444454654644</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q7" s="1" t="n">
-        <v>45646</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>111111</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>4546544456</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q8" s="1" t="n">
-        <v>45646</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>89.99</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q9" s="1" t="n">
-        <v>1515</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1739,18 +1376,18 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="83.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.89"/>
@@ -1760,27 +1397,26 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>64</v>
@@ -1810,12 +1446,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="n">
@@ -1829,39 +1465,39 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>4564648687468</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>4444</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>45</v>
@@ -1874,39 +1510,39 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>5002</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>12</v>
@@ -1919,39 +1555,39 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>182</v>
+        <v>138</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>4020</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>7</v>
@@ -1964,28 +1600,28 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2004,168 +1640,175 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="13.28"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>190</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G2" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>4999999990</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G3" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D4" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>4999999990</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G4" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>3000</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D5" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>9999999999</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G5" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>4444</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>211</v>
+        <v>166</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix -- routes + position for btns import and export
</commit_message>
<xml_diff>
--- a/import_models/models.xlsx
+++ b/import_models/models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Activités" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -126,7 +126,13 @@
     <t xml:space="preserve">Catégorie parente</t>
   </si>
   <si>
+    <t xml:space="preserve">Catégorie pour</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matériel</t>
   </si>
   <si>
     <t xml:space="preserve">Balles de tennis</t>
@@ -543,6 +549,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -641,11 +648,11 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.95"/>
@@ -791,13 +798,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="28.96"/>
   </cols>
@@ -809,47 +816,68 @@
       <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1"/>
+      <c r="C2" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
+      <c r="C3" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1"/>
+      <c r="C6" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -874,11 +902,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.1"/>
@@ -895,42 +923,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>4.99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>4.77</v>
@@ -947,19 +975,19 @@
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>95</v>
@@ -976,19 +1004,19 @@
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>9.95</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>10</v>
@@ -1005,19 +1033,19 @@
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>4.99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>4</v>
@@ -1054,16 +1082,16 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="26.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="61.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="85.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="85.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.68"/>
@@ -1080,72 +1108,72 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>5</v>
@@ -1157,52 +1185,52 @@
         <v>111111</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>4546544456</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q2" s="1" t="n">
         <v>45646</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>10</v>
@@ -1214,52 +1242,52 @@
         <v>89.99</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>1515</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1271,48 +1299,48 @@
         <v>45</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>4564644464</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="Q4" s="1" t="n">
         <v>4545</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>10</v>
@@ -1324,38 +1352,38 @@
         <v>41</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="Q5" s="1" t="n">
         <v>5002</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1408,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.48"/>
@@ -1404,54 +1432,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="n">
@@ -1465,39 +1493,39 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>4564648687468</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>4444</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>45</v>
@@ -1510,39 +1538,39 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>5002</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>12</v>
@@ -1555,39 +1583,39 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>4020</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>7</v>
@@ -1600,28 +1628,28 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1646,7 +1674,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
@@ -1656,159 +1684,159 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="13.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>4999999990</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>4999999990</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>3000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>9999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>4444</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Advancements on error handling
</commit_message>
<xml_diff>
--- a/import_models/models.xlsx
+++ b/import_models/models.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="168">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -45,10 +45,10 @@
     <t xml:space="preserve">Gastropod are awesome !</t>
   </si>
   <si>
-    <t xml:space="preserve">Raquette de Badminton (16.0), machin (6.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hall omnisport Namur, Salle Jen-Jaurès Bruxelles, </t>
+    <t xml:space="preserve">Raquette de Badminton (16.0), machin (6.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hall omnisport Namur, Salle Jen-Jaurès Bruxelles</t>
   </si>
   <si>
     <t xml:space="preserve">Cartes</t>
@@ -57,10 +57,10 @@
     <t xml:space="preserve">On joue aux cartes, c'est trop bien !!!</t>
   </si>
   <si>
-    <t xml:space="preserve">Raquette de Badminton (11.0), Ruban adhésif (3.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hall omnisport Namur, Salle des Morpions Liège, Salle Jen-Jaurès Bruxelles, </t>
+    <t xml:space="preserve">Raquette de Badminton (11.0), Ruban adhésif (3.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hall omnisport Namur, Salle des Morpions Liège, Salle Jen-Jaurès Bruxelles</t>
   </si>
   <si>
     <t xml:space="preserve">Danse de salon</t>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">fchazohcaohcoaihcaohcaoihca</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruban adhésif (6.0), Raquette de Badminton (4.0), machin (2.0), </t>
+    <t xml:space="preserve">Ruban adhésif (6.0), Raquette de Badminton (4.0), machin (2.0)</t>
   </si>
   <si>
     <t xml:space="preserve">Fléchettes</t>
@@ -84,10 +84,10 @@
     <t xml:space="preserve">kdapozkdaopkdapkdada</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruban adhésif (20.0), machin (10.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hall omnisport Namur, Salle des Morpions Liège, </t>
+    <t xml:space="preserve">Ruban adhésif (20.0), machin (10.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hall omnisport Namur, Salle des Morpions Liège</t>
   </si>
   <si>
     <t xml:space="preserve">Handball</t>
@@ -96,10 +96,10 @@
     <t xml:space="preserve">Le hand, c'est du hand :)</t>
   </si>
   <si>
-    <t xml:space="preserve">Raquette de Badminton (10.0), machin (15.0), Ruban adhésif (31.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hall omnisport Namur, </t>
+    <t xml:space="preserve">Raquette de Badminton (10.0), machin (15.0), Ruban adhésif (31.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hall omnisport Namur</t>
   </si>
   <si>
     <t xml:space="preserve">Paintball</t>
@@ -108,7 +108,7 @@
     <t xml:space="preserve">Mega trop bien le paintball !!!</t>
   </si>
   <si>
-    <t xml:space="preserve">machin (10.0), Raquette de Badminton (6.0), </t>
+    <t xml:space="preserve">machin (10.0), Raquette de Badminton (6.0)</t>
   </si>
   <si>
     <t xml:space="preserve">Ping-Pong</t>
@@ -117,10 +117,10 @@
     <t xml:space="preserve">dohdoahdoazhdoahodada</t>
   </si>
   <si>
-    <t xml:space="preserve">Projecteur multicouleur (4.0), Ruban adhésif (8.0), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salle des Morpions Liège, </t>
+    <t xml:space="preserve">Projecteur multicouleur (4.0), Ruban adhésif (8.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salle des Morpions Liège</t>
   </si>
   <si>
     <t xml:space="preserve">Catégorie parente</t>
@@ -132,12 +132,12 @@
     <t xml:space="preserve">Balles</t>
   </si>
   <si>
+    <t xml:space="preserve">Balles de tennis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matériel</t>
   </si>
   <si>
-    <t xml:space="preserve">Balles de tennis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Projecteur</t>
   </si>
   <si>
@@ -264,13 +264,10 @@
     <t xml:space="preserve">20/04/2021, à 17:45</t>
   </si>
   <si>
-    <t xml:space="preserve">Salle des Morpions Liège</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartes (5), Danse de salon (10), Football (20), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">machin (3.0), Projecteur multicouleur (10.0), Ruban adhésif (40.0), </t>
+    <t xml:space="preserve">Cartes (5), Danse de salon (10), Football (20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machin (3.0), Projecteur multicouleur (10.0), Ruban adhésif (40.0)</t>
   </si>
   <si>
     <t xml:space="preserve">dhaidhaiuhd</t>
@@ -303,10 +300,10 @@
     <t xml:space="preserve">14/03/2031, à 00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">Cartes (4), Danse de salon (8), Fléchettes (5), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projecteur multicouleur (30.0), Ruban adhésif (120.0), </t>
+    <t xml:space="preserve">Cartes (4), Danse de salon (8), Fléchettes (5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projecteur multicouleur (30.0), Ruban adhésif (120.0)</t>
   </si>
   <si>
     <t xml:space="preserve">Boubouche</t>
@@ -339,9 +336,6 @@
     <t xml:space="preserve">20/03/2041, à 21:19</t>
   </si>
   <si>
-    <t xml:space="preserve">Hall omnisport Namur</t>
-  </si>
-  <si>
     <t xml:space="preserve">hdizhdadaz</t>
   </si>
   <si>
@@ -372,10 +366,10 @@
     <t xml:space="preserve">18/03/2041, à 22:24</t>
   </si>
   <si>
-    <t xml:space="preserve">Badminton (10), Cartes (5), Handball (3), </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruban adhésif (25.0), Projecteur multicouleur (10.0), </t>
+    <t xml:space="preserve">Badminton (10), Cartes (5), Handball (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruban adhésif (25.0), Projecteur multicouleur (10.0)</t>
   </si>
   <si>
     <t xml:space="preserve">Bastin</t>
@@ -438,13 +432,13 @@
     <t xml:space="preserve">dajzopdajdajda</t>
   </si>
   <si>
-    <t xml:space="preserve">Danse de salon, Handball, Cartes, Football, Badminton, Paintball, </t>
+    <t xml:space="preserve">Danse de salon, Handball, Cartes, Football, Badminton, Paintball</t>
   </si>
   <si>
     <t xml:space="preserve">bastincyriel@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Danse de salon, Cartes, Football, Ping-Pong, </t>
+    <t xml:space="preserve">Danse de salon, Cartes, Football, Ping-Pong</t>
   </si>
   <si>
     <t xml:space="preserve">LaLouche</t>
@@ -468,7 +462,7 @@
     <t xml:space="preserve">Salle Jen-Jaurès Bruxelles</t>
   </si>
   <si>
-    <t xml:space="preserve">Danse de salon, Cartes, Badminton, </t>
+    <t xml:space="preserve">Danse de salon, Cartes, Badminton</t>
   </si>
   <si>
     <t xml:space="preserve">Molimo</t>
@@ -652,12 +646,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="84.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="95.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="92.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,12 +795,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="28.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,28 +811,26 @@
       <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="0" t="s">
-        <v>35</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>35</v>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,8 +838,8 @@
         <v>37</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="0" t="s">
-        <v>35</v>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,8 +849,8 @@
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>35</v>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,8 +858,8 @@
         <v>39</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="0" t="s">
-        <v>35</v>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,8 +869,8 @@
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>35</v>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -899,10 +892,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.92"/>
@@ -944,7 +937,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -955,7 +948,7 @@
         <v>4.99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>50</v>
@@ -1082,7 +1075,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="26.55"/>
@@ -1090,8 +1083,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="61.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="85.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="59.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="83.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.68"/>
@@ -1185,52 +1178,52 @@
         <v>111111</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>4546544456</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="Q2" s="1" t="n">
         <v>45646</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>10</v>
@@ -1242,52 +1235,52 @@
         <v>89.99</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>1515</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1299,48 +1292,48 @@
         <v>45</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>4564644464</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q4" s="1" t="n">
         <v>4545</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>10</v>
@@ -1352,38 +1345,38 @@
         <v>41</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="Q5" s="1" t="n">
         <v>5002</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1408,11 +1401,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="83.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.89"/>
@@ -1432,19 +1425,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>66</v>
@@ -1476,10 +1469,10 @@
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="n">
@@ -1493,39 +1486,39 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>4564648687468</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>4444</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>45</v>
@@ -1538,39 +1531,39 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>5002</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>12</v>
@@ -1583,39 +1576,39 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>4020</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>7</v>
@@ -1628,28 +1621,28 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1674,7 +1667,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
@@ -1689,7 +1682,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>66</v>
@@ -1721,32 +1714,32 @@
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,28 +1748,28 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>4999999990</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,28 +1778,28 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>4999999990</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>3000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,28 +1808,28 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>9999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>4444</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements on import functionality
</commit_message>
<xml_diff>
--- a/import_models/models.xlsx
+++ b/import_models/models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Activités" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="168">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -132,10 +132,10 @@
     <t xml:space="preserve">Balles</t>
   </si>
   <si>
+    <t xml:space="preserve">Matériel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balles de tennis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matériel</t>
   </si>
   <si>
     <t xml:space="preserve">Projecteur</t>
@@ -643,10 +643,10 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.95"/>
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -682,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -696,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -794,11 +794,11 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.52"/>
@@ -820,26 +820,28 @@
         <v>34</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,16 +852,16 @@
         <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +872,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -892,10 +894,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.92"/>
@@ -966,7 +968,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -995,7 +997,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -1072,10 +1074,10 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="26.55"/>
@@ -1155,7 +1157,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1212,7 +1214,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -1269,7 +1271,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>99</v>
       </c>
@@ -1322,7 +1324,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>109</v>
       </c>
@@ -1398,10 +1400,10 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.48"/>
@@ -1467,7 +1469,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>127</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1555,7 +1557,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>144</v>
       </c>
@@ -1663,11 +1665,11 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
@@ -1712,7 +1714,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>153</v>
       </c>
@@ -1742,7 +1744,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -1802,7 +1804,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Fix some errors on category import
</commit_message>
<xml_diff>
--- a/import_models/models.xlsx
+++ b/import_models/models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Activités" sheetId="1" state="visible" r:id="rId2"/>
@@ -646,7 +646,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.95"/>
@@ -794,11 +794,11 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.52"/>
@@ -844,7 +844,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -897,7 +897,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.92"/>
@@ -1077,7 +1077,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="26.55"/>
@@ -1403,7 +1403,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.48"/>
@@ -1665,11 +1665,11 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>

</xml_diff>